<commit_message>
Creación del método encontrarMSC
</commit_message>
<xml_diff>
--- a/src/main/java/algestudiante/p5/P5_UO277876.xlsx
+++ b/src/main/java/algestudiante/p5/P5_UO277876.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\infer\git\alg_AunonAndreaUO277876\src\main\java\algestudiante\p5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E4D23F-01AC-4377-AA64-20FEF48828EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8FC31D-ACBD-409B-A96D-6E077A1424FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>nVeces</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>O(nlogn)</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
   <si>
     <t>t(Prog. Dinámica)</t>
@@ -411,7 +408,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Prog. Dinámica'!$C$2</c:f>
+              <c:f>'Prog. Dinámica'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -423,7 +420,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -446,138 +443,138 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
+              <c:f>'Prog. Dinámica'!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>102400</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>204800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>409600</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>819200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1638400</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3276800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6553600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13107200</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26214400</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>52428800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>'Prog. Dinámica'!$B$3:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>800</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12800</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>102400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>204800</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>409600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>819200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1638400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3276800</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6553600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13107200</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26214400</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>52428800</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Prog. Dinámica'!$C$3:$C$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>1.7100000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.6000000000000002E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.0800000000000003E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.1640000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.4229999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.8630000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.5499999999999995E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.9602999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.8151999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7.6614000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.15032899999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.29681000000000002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.60407</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.27176</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.6665000000000001</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.3940999999999999</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>10.739599999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>22.338999999999999</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44.255000000000003</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>89.495000000000005</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -841,7 +838,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Prog. Dinámica'!$D$2</c:f>
+              <c:f>'Prog. Dinámica'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -853,7 +850,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="FFC000"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -876,138 +873,138 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Prog. Dinámica'!$B$3:$B$22</c:f>
+              <c:f>'Prog. Dinámica'!$E$3:$E$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>400</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>800</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1600</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3200</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6400</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12800</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25600</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51200</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>102400</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>204800</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>409600</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>819200</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1638400</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3276800</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6553600</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13107200</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26214400</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>52428800</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Prog. Dinámica'!$D$3:$D$22</c:f>
+              <c:f>'Prog. Dinámica'!$F$3:$F$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>2.1700000000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5999999999999999E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.9500000000000005E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7430000000000001E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.7310000000000003E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.424E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.17363000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.35206999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.82206000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6734800000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0482999999999998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.5076000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.625599999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23.931000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>46.341999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>83.436000000000007</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>150.39400000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>259.54000000000002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>530.09</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1535.35</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2699,14 +2696,14 @@
   <dimension ref="A2:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.21875" customWidth="1"/>
     <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" customWidth="1"/>
     <col min="5" max="5" width="18.109375" customWidth="1"/>
     <col min="6" max="6" width="19.21875" customWidth="1"/>
@@ -2714,20 +2711,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>18</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>1</v>
@@ -2738,21 +2738,24 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="16">
+        <v>100</v>
+      </c>
+      <c r="B3" s="19" t="e">
+        <f>171/M6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="16">
-        <v>100</v>
-      </c>
-      <c r="C3" s="19">
-        <f>171/N6</f>
-        <v>1.7100000000000001E-4</v>
-      </c>
-      <c r="D3" s="19">
-        <f>217/N7</f>
-        <v>2.1700000000000001E-3</v>
-      </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="16">
+        <v>2</v>
+      </c>
+      <c r="F3" s="19" t="e">
+        <f>217/P7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G3" s="23" t="s">
         <v>6</v>
       </c>
       <c r="J3" s="6" t="s">
@@ -2764,19 +2767,22 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="16">
+      <c r="A4" s="16">
         <v>200</v>
       </c>
-      <c r="C4" s="19">
-        <f>360/N6</f>
-        <v>3.6000000000000002E-4</v>
-      </c>
-      <c r="D4" s="19">
-        <f>360/N7</f>
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="E4" s="23"/>
+      <c r="B4" s="19" t="e">
+        <f>360/M6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="E4" s="16">
+        <v>4</v>
+      </c>
+      <c r="F4" s="19" t="e">
+        <f>360/P7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" s="23"/>
       <c r="J4" s="8" t="s">
         <v>3</v>
       </c>
@@ -2786,324 +2792,378 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="16">
+      <c r="A5" s="16">
         <v>400</v>
       </c>
-      <c r="C5" s="19">
-        <f>608/N6</f>
-        <v>6.0800000000000003E-4</v>
-      </c>
-      <c r="D5" s="19">
-        <f>795/N7</f>
-        <v>7.9500000000000005E-3</v>
-      </c>
-      <c r="E5" s="23"/>
+      <c r="B5" s="19" t="e">
+        <f>608/M6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="E5" s="16">
+        <v>6</v>
+      </c>
+      <c r="F5" s="19" t="e">
+        <f>795/P7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" s="23"/>
       <c r="N5" s="2">
         <v>10000000</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="16">
+      <c r="A6" s="16">
         <v>800</v>
       </c>
-      <c r="C6" s="19">
-        <f>1164/N6</f>
-        <v>1.1640000000000001E-3</v>
-      </c>
-      <c r="D6" s="19">
-        <f>1743/N7</f>
-        <v>1.7430000000000001E-2</v>
-      </c>
-      <c r="E6" s="23"/>
+      <c r="B6" s="19" t="e">
+        <f>1164/M6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="E6" s="16">
+        <v>8</v>
+      </c>
+      <c r="F6" s="19" t="e">
+        <f>1743/P7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G6" s="23"/>
       <c r="N6" s="2">
         <v>1000000</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="16">
+      <c r="A7" s="16">
         <v>1600</v>
       </c>
-      <c r="C7" s="19">
-        <f>2423/N6</f>
-        <v>2.4229999999999998E-3</v>
-      </c>
-      <c r="D7" s="19">
-        <f>3731/N7</f>
-        <v>3.7310000000000003E-2</v>
-      </c>
-      <c r="E7" s="23"/>
+      <c r="B7" s="19" t="e">
+        <f>2423/M6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="E7" s="16">
+        <v>10</v>
+      </c>
+      <c r="F7" s="19" t="e">
+        <f>3731/P7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7" s="23"/>
       <c r="N7" s="3">
         <v>100000</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="16">
+      <c r="A8" s="16">
         <v>3200</v>
       </c>
-      <c r="C8" s="19">
-        <f>4863/N6</f>
-        <v>4.8630000000000001E-3</v>
-      </c>
-      <c r="D8" s="19">
-        <f>7424/N7</f>
-        <v>7.424E-2</v>
-      </c>
-      <c r="E8" s="23"/>
+      <c r="B8" s="19" t="e">
+        <f>4863/M6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="E8" s="16">
+        <v>12</v>
+      </c>
+      <c r="F8" s="19" t="e">
+        <f>7424/P7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G8" s="23"/>
       <c r="N8" s="2">
         <v>10000</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="16">
+      <c r="A9" s="16">
         <v>6400</v>
       </c>
-      <c r="C9" s="19">
-        <f>9550/N6</f>
-        <v>9.5499999999999995E-3</v>
-      </c>
-      <c r="D9" s="19">
-        <f>17363/N7</f>
-        <v>0.17363000000000001</v>
-      </c>
-      <c r="E9" s="23"/>
+      <c r="B9" s="19" t="e">
+        <f>9550/M6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="E9" s="16">
+        <v>14</v>
+      </c>
+      <c r="F9" s="19" t="e">
+        <f>17363/P7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G9" s="23"/>
       <c r="N9" s="14">
         <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16">
+      <c r="A10" s="16">
         <v>12800</v>
       </c>
-      <c r="C10" s="19">
-        <f>19603/N6</f>
-        <v>1.9602999999999999E-2</v>
-      </c>
-      <c r="D10" s="19">
-        <f>35207/N7</f>
-        <v>0.35206999999999999</v>
-      </c>
-      <c r="E10" s="23"/>
+      <c r="B10" s="19" t="e">
+        <f>19603/M6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="E10" s="16">
+        <v>16</v>
+      </c>
+      <c r="F10" s="19" t="e">
+        <f>35207/P7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G10" s="23"/>
       <c r="N10" s="14">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="16">
+      <c r="A11" s="16">
         <v>25600</v>
       </c>
-      <c r="C11" s="19">
-        <f>38152/N6</f>
-        <v>3.8151999999999998E-2</v>
-      </c>
-      <c r="D11" s="19">
-        <f>82206/N7</f>
-        <v>0.82206000000000001</v>
-      </c>
-      <c r="E11" s="23"/>
+      <c r="B11" s="19" t="e">
+        <f>38152/M6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="E11" s="16">
+        <v>18</v>
+      </c>
+      <c r="F11" s="19" t="e">
+        <f>82206/P7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11" s="23"/>
       <c r="N11" s="14">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16">
+      <c r="A12" s="16">
         <v>51200</v>
       </c>
-      <c r="C12" s="19">
-        <f>76614/N6</f>
-        <v>7.6614000000000002E-2</v>
-      </c>
-      <c r="D12" s="19">
-        <f>167348/N7</f>
-        <v>1.6734800000000001</v>
-      </c>
-      <c r="E12" s="23"/>
+      <c r="B12" s="19" t="e">
+        <f>76614/M6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="E12" s="16">
+        <v>20</v>
+      </c>
+      <c r="F12" s="19" t="e">
+        <f>167348/P7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G12" s="23"/>
       <c r="N12" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16">
+      <c r="A13" s="16">
         <v>102400</v>
       </c>
-      <c r="C13" s="19">
-        <f>150329/N6</f>
-        <v>0.15032899999999999</v>
-      </c>
-      <c r="D13" s="19">
-        <f>30483/N8</f>
-        <v>3.0482999999999998</v>
-      </c>
-      <c r="E13" s="23" t="s">
+      <c r="B13" s="19" t="e">
+        <f>150329/M6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="E13" s="16">
+        <v>22</v>
+      </c>
+      <c r="F13" s="19" t="e">
+        <f>30483/P8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" s="23" t="s">
         <v>7</v>
-      </c>
-      <c r="K13" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="16">
+        <v>204800</v>
+      </c>
+      <c r="B14" s="19" t="e">
+        <f>29681/M7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="16">
-        <v>204800</v>
-      </c>
-      <c r="C14" s="19">
-        <f>29681/N7</f>
-        <v>0.29681000000000002</v>
-      </c>
-      <c r="D14" s="19">
-        <f>75076/N8</f>
-        <v>7.5076000000000001</v>
-      </c>
-      <c r="E14" s="23"/>
+      <c r="E14" s="16">
+        <v>24</v>
+      </c>
+      <c r="F14" s="19" t="e">
+        <f>75076/P8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="16">
+      <c r="A15" s="16">
         <v>409600</v>
       </c>
-      <c r="C15" s="19">
-        <f>60407/N7</f>
-        <v>0.60407</v>
-      </c>
-      <c r="D15" s="19">
-        <f>166256/N8</f>
-        <v>16.625599999999999</v>
-      </c>
-      <c r="E15" s="23"/>
+      <c r="B15" s="19" t="e">
+        <f>60407/M7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="E15" s="16">
+        <v>26</v>
+      </c>
+      <c r="F15" s="19" t="e">
+        <f>166256/P8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="16">
+      <c r="A16" s="16">
         <v>819200</v>
       </c>
-      <c r="C16" s="19">
-        <f>127176/N7</f>
-        <v>1.27176</v>
-      </c>
-      <c r="D16" s="19">
-        <f>23931/N9</f>
-        <v>23.931000000000001</v>
-      </c>
-      <c r="E16" s="23" t="s">
+      <c r="B16" s="19" t="e">
+        <f>127176/M7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="E16" s="16">
+        <v>28</v>
+      </c>
+      <c r="F16" s="19" t="e">
+        <f>23931/P9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" s="23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>1638400</v>
+      </c>
+      <c r="B17" s="19" t="e">
+        <f>26665/M8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="16">
-        <v>1638400</v>
-      </c>
-      <c r="C17" s="19">
-        <f>26665/N8</f>
-        <v>2.6665000000000001</v>
-      </c>
-      <c r="D17" s="19">
-        <f>46342/N9</f>
-        <v>46.341999999999999</v>
-      </c>
-      <c r="E17" s="23"/>
+      <c r="E17" s="16">
+        <v>30</v>
+      </c>
+      <c r="F17" s="19" t="e">
+        <f>46342/P9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" s="23"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
-      <c r="B18" s="16">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
         <v>3276800</v>
       </c>
-      <c r="C18" s="19">
-        <f>53941/N8</f>
-        <v>5.3940999999999999</v>
-      </c>
-      <c r="D18" s="19">
-        <f>83436/N9</f>
-        <v>83.436000000000007</v>
-      </c>
-      <c r="E18" s="23"/>
+      <c r="B18" s="19" t="e">
+        <f>53941/M8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="E18" s="16">
+        <v>32</v>
+      </c>
+      <c r="F18" s="19" t="e">
+        <f>83436/P9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G18" s="23"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="18">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="18">
         <v>6553600</v>
       </c>
-      <c r="C19" s="19">
-        <f>107396/N8</f>
-        <v>10.739599999999999</v>
-      </c>
-      <c r="D19" s="19">
-        <f>150394/N9</f>
-        <v>150.39400000000001</v>
-      </c>
-      <c r="E19" s="23" t="s">
+      <c r="B19" s="19" t="e">
+        <f>107396/M8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="E19" s="16">
+        <v>34</v>
+      </c>
+      <c r="F19" s="19" t="e">
+        <f>150394/P9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" s="23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="18">
+        <v>13107200</v>
+      </c>
+      <c r="B20" s="19" t="e">
+        <f>22339/M9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="18">
-        <v>13107200</v>
-      </c>
-      <c r="C20" s="19">
-        <f>22339/N9</f>
-        <v>22.338999999999999</v>
-      </c>
-      <c r="D20" s="19">
-        <f>25954/N10</f>
-        <v>259.54000000000002</v>
-      </c>
-      <c r="E20" s="7"/>
+      <c r="E20" s="16">
+        <v>36</v>
+      </c>
+      <c r="F20" s="19" t="e">
+        <f>25954/P10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="18">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="18">
         <v>26214400</v>
       </c>
-      <c r="C21" s="19">
-        <f>44255/N9</f>
-        <v>44.255000000000003</v>
-      </c>
-      <c r="D21" s="19">
-        <f>53009/N10</f>
-        <v>530.09</v>
-      </c>
-      <c r="E21" s="7"/>
+      <c r="B21" s="19" t="e">
+        <f>44255/M9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="E21" s="16">
+        <v>38</v>
+      </c>
+      <c r="F21" s="19" t="e">
+        <f>53009/P10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="20">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="20">
         <v>52428800</v>
       </c>
-      <c r="C22" s="21">
-        <f>89495/N9</f>
-        <v>89.495000000000005</v>
-      </c>
-      <c r="D22" s="21">
-        <f>153535/N10</f>
-        <v>1535.35</v>
-      </c>
-      <c r="E22" s="24" t="s">
+      <c r="B22" s="21" t="e">
+        <f>89495/M9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="E22" s="16">
+        <v>40</v>
+      </c>
+      <c r="F22" s="21" t="e">
+        <f>153535/P10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="25" t="s">
+        <v>11</v>
+      </c>
       <c r="B23" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="25" t="s">
+      <c r="F23" s="25" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Medición de tiempos realizada
</commit_message>
<xml_diff>
--- a/src/main/java/algestudiante/p5/P5_UO277876.xlsx
+++ b/src/main/java/algestudiante/p5/P5_UO277876.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\infer\git\alg_AunonAndreaUO277876\src\main\java\algestudiante\p5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8FC31D-ACBD-409B-A96D-6E077A1424FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F4EAAC-1C06-4510-9712-C14A1F15F3AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>nVeces</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>n</t>
-  </si>
-  <si>
-    <t>nVeces = 1000000</t>
   </si>
   <si>
     <t>nVeces = 100000</t>
@@ -88,6 +85,15 @@
   </si>
   <si>
     <t>nVeces (DV)</t>
+  </si>
+  <si>
+    <t>nVeces = 1</t>
+  </si>
+  <si>
+    <t>NOTA:</t>
+  </si>
+  <si>
+    <t>Cuando pongo nVeces = 100, el ordenador deja de funcionar bien</t>
   </si>
 </sst>
 </file>
@@ -144,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -271,11 +277,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -303,21 +322,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,10 +459,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Prog. Dinámica'!$A$3:$A$22</c:f>
+              <c:f>'Prog. Dinámica'!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -465,116 +481,32 @@
                 <c:pt idx="5">
                   <c:v>3200</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>6400</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12800</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>25600</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>51200</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>102400</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>204800</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>409600</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>819200</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1638400</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3276800</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>6553600</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>13107200</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>26214400</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>52428800</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Prog. Dinámica'!$B$3:$B$22</c:f>
+              <c:f>'Prog. Dinámica'!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.036</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2.3860000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>6.9880000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>25.533999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>123.77500000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>635.21699999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -850,7 +782,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FFC000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -873,10 +805,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Prog. Dinámica'!$E$3:$E$22</c:f>
+              <c:f>'Prog. Dinámica'!$E$3:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -898,113 +830,35 @@
                 <c:pt idx="6">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>40</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Prog. Dinámica'!$F$3:$F$22</c:f>
+              <c:f>'Prog. Dinámica'!$F$3:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.6619999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.43482999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>14.431800000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>426.66</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>12597.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>390211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2321,14 +2175,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>937260</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2357,16 +2211,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1226820</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2693,18 +2547,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50AC779-C55D-4822-8A6D-58AA05F2A758}">
-  <dimension ref="A2:N23"/>
+  <dimension ref="A2:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.21875" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
     <col min="5" max="5" width="18.109375" customWidth="1"/>
     <col min="6" max="6" width="19.21875" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
@@ -2715,19 +2569,19 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>1</v>
@@ -2741,22 +2595,22 @@
       <c r="A3" s="16">
         <v>100</v>
       </c>
-      <c r="B3" s="19" t="e">
-        <f>171/M6</f>
-        <v>#DIV/0!</v>
+      <c r="B3" s="20">
+        <f>1036/N9</f>
+        <v>1.036</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" s="16">
         <v>2</v>
       </c>
-      <c r="F3" s="19" t="e">
-        <f>217/P7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>6</v>
+      <c r="F3" s="20">
+        <f>200/N7</f>
+        <v>2E-3</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>2</v>
@@ -2770,19 +2624,19 @@
       <c r="A4" s="16">
         <v>200</v>
       </c>
-      <c r="B4" s="19" t="e">
-        <f>360/M6</f>
-        <v>#DIV/0!</v>
+      <c r="B4" s="20">
+        <f>2386/N9</f>
+        <v>2.3860000000000001</v>
       </c>
       <c r="C4" s="13"/>
       <c r="E4" s="16">
         <v>4</v>
       </c>
-      <c r="F4" s="19" t="e">
-        <f>360/P7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" s="23"/>
+      <c r="F4" s="20">
+        <f>1662/N7</f>
+        <v>1.6619999999999999E-2</v>
+      </c>
+      <c r="G4" s="13"/>
       <c r="J4" s="8" t="s">
         <v>3</v>
       </c>
@@ -2795,19 +2649,19 @@
       <c r="A5" s="16">
         <v>400</v>
       </c>
-      <c r="B5" s="19" t="e">
-        <f>608/M6</f>
-        <v>#DIV/0!</v>
+      <c r="B5" s="20">
+        <f>6988/N9</f>
+        <v>6.9880000000000004</v>
       </c>
       <c r="C5" s="13"/>
       <c r="E5" s="16">
         <v>6</v>
       </c>
-      <c r="F5" s="19" t="e">
-        <f>795/P7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G5" s="23"/>
+      <c r="F5" s="20">
+        <f>43483/N7</f>
+        <v>0.43482999999999999</v>
+      </c>
+      <c r="G5" s="13"/>
       <c r="N5" s="2">
         <v>10000000</v>
       </c>
@@ -2816,19 +2670,21 @@
       <c r="A6" s="16">
         <v>800</v>
       </c>
-      <c r="B6" s="19" t="e">
-        <f>1164/M6</f>
-        <v>#DIV/0!</v>
+      <c r="B6" s="20">
+        <f>25534/N9</f>
+        <v>25.533999999999999</v>
       </c>
       <c r="C6" s="13"/>
       <c r="E6" s="16">
         <v>8</v>
       </c>
-      <c r="F6" s="19" t="e">
-        <f>1743/P7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G6" s="23"/>
+      <c r="F6" s="20">
+        <f>144318/N8</f>
+        <v>14.431800000000001</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>6</v>
+      </c>
       <c r="N6" s="2">
         <v>1000000</v>
       </c>
@@ -2837,334 +2693,96 @@
       <c r="A7" s="16">
         <v>1600</v>
       </c>
-      <c r="B7" s="19" t="e">
-        <f>2423/M6</f>
-        <v>#DIV/0!</v>
+      <c r="B7" s="20">
+        <f>123775/N9</f>
+        <v>123.77500000000001</v>
       </c>
       <c r="C7" s="13"/>
       <c r="E7" s="16">
         <v>10</v>
       </c>
-      <c r="F7" s="19" t="e">
-        <f>3731/P7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" s="23"/>
+      <c r="F7" s="20">
+        <f>42666/N10</f>
+        <v>426.66</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="N7" s="3">
         <v>100000</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="16">
+      <c r="A8" s="18">
         <v>3200</v>
       </c>
-      <c r="B8" s="19" t="e">
-        <f>4863/M6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C8" s="13"/>
+      <c r="B8" s="21">
+        <f>635217/N9</f>
+        <v>635.21699999999998</v>
+      </c>
+      <c r="C8" s="19"/>
       <c r="E8" s="16">
         <v>12</v>
       </c>
-      <c r="F8" s="19" t="e">
-        <f>7424/P7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G8" s="23"/>
+      <c r="F8" s="20">
+        <f>125979/N11</f>
+        <v>12597.9</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>9</v>
+      </c>
       <c r="N8" s="2">
         <v>10000</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="16">
-        <v>6400</v>
-      </c>
-      <c r="B9" s="19" t="e">
-        <f>9550/M6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="E9" s="16">
+      <c r="A9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="E9" s="18">
         <v>14</v>
       </c>
-      <c r="F9" s="19" t="e">
-        <f>17363/P7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G9" s="23"/>
+      <c r="F9" s="21">
+        <f>390211/N12</f>
+        <v>390211</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="N9" s="14">
         <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="16">
-        <v>12800</v>
-      </c>
-      <c r="B10" s="19" t="e">
-        <f>19603/M6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="E10" s="16">
-        <v>16</v>
-      </c>
-      <c r="F10" s="19" t="e">
-        <f>35207/P7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G10" s="23"/>
+      <c r="A10" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="E10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="N10" s="14">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="16">
-        <v>25600</v>
-      </c>
-      <c r="B11" s="19" t="e">
-        <f>38152/M6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="E11" s="16">
-        <v>18</v>
-      </c>
-      <c r="F11" s="19" t="e">
-        <f>82206/P7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G11" s="23"/>
       <c r="N11" s="14">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="16">
-        <v>51200</v>
-      </c>
-      <c r="B12" s="19" t="e">
-        <f>76614/M6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="E12" s="16">
-        <v>20</v>
-      </c>
-      <c r="F12" s="19" t="e">
-        <f>167348/P7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G12" s="23"/>
       <c r="N12" s="14">
         <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="16">
-        <v>102400</v>
-      </c>
-      <c r="B13" s="19" t="e">
-        <f>150329/M6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="E13" s="16">
-        <v>22</v>
-      </c>
-      <c r="F13" s="19" t="e">
-        <f>30483/P8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="16">
-        <v>204800</v>
-      </c>
-      <c r="B14" s="19" t="e">
-        <f>29681/M7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="16">
-        <v>24</v>
-      </c>
-      <c r="F14" s="19" t="e">
-        <f>75076/P8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G14" s="23"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="16">
-        <v>409600</v>
-      </c>
-      <c r="B15" s="19" t="e">
-        <f>60407/M7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="E15" s="16">
-        <v>26</v>
-      </c>
-      <c r="F15" s="19" t="e">
-        <f>166256/P8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G15" s="23"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="16">
-        <v>819200</v>
-      </c>
-      <c r="B16" s="19" t="e">
-        <f>127176/M7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="E16" s="16">
-        <v>28</v>
-      </c>
-      <c r="F16" s="19" t="e">
-        <f>23931/P9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="16">
-        <v>1638400</v>
-      </c>
-      <c r="B17" s="19" t="e">
-        <f>26665/M8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="16">
-        <v>30</v>
-      </c>
-      <c r="F17" s="19" t="e">
-        <f>46342/P9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G17" s="23"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="16">
-        <v>3276800</v>
-      </c>
-      <c r="B18" s="19" t="e">
-        <f>53941/M8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="E18" s="16">
-        <v>32</v>
-      </c>
-      <c r="F18" s="19" t="e">
-        <f>83436/P9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G18" s="23"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="18">
-        <v>6553600</v>
-      </c>
-      <c r="B19" s="19" t="e">
-        <f>107396/M8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="E19" s="16">
-        <v>34</v>
-      </c>
-      <c r="F19" s="19" t="e">
-        <f>150394/P9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="18">
-        <v>13107200</v>
-      </c>
-      <c r="B20" s="19" t="e">
-        <f>22339/M9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="16">
-        <v>36</v>
-      </c>
-      <c r="F20" s="19" t="e">
-        <f>25954/P10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="18">
-        <v>26214400</v>
-      </c>
-      <c r="B21" s="19" t="e">
-        <f>44255/M9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="E21" s="16">
-        <v>38</v>
-      </c>
-      <c r="F21" s="19" t="e">
-        <f>53009/P10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="20">
-        <v>52428800</v>
-      </c>
-      <c r="B22" s="21" t="e">
-        <f>89495/M9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="E22" s="16">
-        <v>40</v>
-      </c>
-      <c r="F22" s="21" t="e">
-        <f>153535/P10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G22" s="24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="25" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrección en las complejidades para pasarlo a pdf
</commit_message>
<xml_diff>
--- a/src/main/java/algestudiante/p5/P5_UO277876.xlsx
+++ b/src/main/java/algestudiante/p5/P5_UO277876.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\infer\git\alg_AunonAndreaUO277876\src\main\java\algestudiante\p5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F4EAAC-1C06-4510-9712-C14A1F15F3AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4609095B-B2AF-4EFC-99CC-269A7FF3BB7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
   </bookViews>
@@ -69,12 +69,6 @@
     <t>Complejidad:</t>
   </si>
   <si>
-    <t>O(n)</t>
-  </si>
-  <si>
-    <t>O(nlogn)</t>
-  </si>
-  <si>
     <t>t(Prog. Dinámica)</t>
   </si>
   <si>
@@ -94,6 +88,12 @@
   </si>
   <si>
     <t>Cuando pongo nVeces = 100, el ordenador deja de funcionar bien</t>
+  </si>
+  <si>
+    <t>O(n^2)</t>
+  </si>
+  <si>
+    <t>O(2^(n))</t>
   </si>
 </sst>
 </file>
@@ -2550,7 +2550,7 @@
   <dimension ref="A2:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2569,19 +2569,19 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>15</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>1</v>
@@ -2740,7 +2740,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C9" s="16"/>
       <c r="E9" s="18">
@@ -2751,7 +2751,7 @@
         <v>390211</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="N9" s="14">
         <v>1000</v>
@@ -2759,17 +2759,17 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="16"/>
       <c r="E10" s="17" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N10" s="14">
         <v>100</v>

</xml_diff>